<commit_message>
chap 7 laboral TD
</commit_message>
<xml_diff>
--- a/td_paises.xlsx
+++ b/td_paises.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Google Drive\Uninorte\Uninorte-docencia\bookdown\intro_eco_col\int_eco_co_notas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B81E40-C977-47F3-91BF-43B67889C617}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AD43D4-6B5D-49F5-96F2-8CEB93793F17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Series - Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$W$189</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$X$188</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1662,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="V41" sqref="V41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15783,6 +15783,7 @@
       <c r="B193" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:X188" xr:uid="{4C5036A0-FD8A-4C3B-80D5-14368ACAB36B}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>